<commit_message>
reorg of functions in subfolder
</commit_message>
<xml_diff>
--- a/templates/input_2photon.xlsx
+++ b/templates/input_2photon.xlsx
@@ -1,22 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\nwb\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF5B5272-1912-4BDC-85AE-F7B3518A2E0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF3F1CBC-75F2-4900-8651-0FB3241348A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31755" yWindow="3825" windowWidth="28800" windowHeight="15345" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="auto" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -25,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="64">
   <si>
     <t>session_id</t>
   </si>
@@ -33,9 +44,6 @@
     <t>subject_id</t>
   </si>
   <si>
-    <t>age</t>
-  </si>
-  <si>
     <t>subject_description</t>
   </si>
   <si>
@@ -60,33 +68,15 @@
     <t>session_description</t>
   </si>
   <si>
-    <t>src_folder_directory</t>
-  </si>
-  <si>
     <t>stimulus_notes_include</t>
   </si>
   <si>
     <t>stimulus_notes_paradigm</t>
   </si>
   <si>
-    <t>stimulus_notes_direct_electrical_stimulation</t>
-  </si>
-  <si>
-    <t>stimulus_notes_direct_electrical_stimulation_paradigm</t>
-  </si>
-  <si>
-    <t>pharmacology_notes_anesthetized_during_recording</t>
-  </si>
-  <si>
-    <t>pharmacology</t>
-  </si>
-  <si>
     <t>anesthesia_acute_chronic</t>
   </si>
   <si>
-    <t>anesthesia_chronic_days_post_admin</t>
-  </si>
-  <si>
     <t>device_name</t>
   </si>
   <si>
@@ -96,42 +86,6 @@
     <t>device_manufacturer</t>
   </si>
   <si>
-    <t>optical_channel_name</t>
-  </si>
-  <si>
-    <t>optical_channel_description</t>
-  </si>
-  <si>
-    <t>optical_channel_emission_lambda</t>
-  </si>
-  <si>
-    <t>image_stack_name</t>
-  </si>
-  <si>
-    <t>image_stack_imaging_rate</t>
-  </si>
-  <si>
-    <t>image_stack_description</t>
-  </si>
-  <si>
-    <t>image_stack_exitation_lambda</t>
-  </si>
-  <si>
-    <t>image_stack_indicator</t>
-  </si>
-  <si>
-    <t>image_stack_location</t>
-  </si>
-  <si>
-    <t>image_stack_grid_spacing</t>
-  </si>
-  <si>
-    <t>image_stack_grid_spacing_unit</t>
-  </si>
-  <si>
-    <t>ROI2_SplC_9x_stk_avg100_670_690um_zernike60_00001.tif</t>
-  </si>
-  <si>
     <t>SST-tdTomato-1</t>
   </si>
   <si>
@@ -153,48 +107,9 @@
     <t>C57BL/6</t>
   </si>
   <si>
-    <t>Fig 17</t>
-  </si>
-  <si>
-    <t>Figure 17/ROI2_SplC_9x_stk_avg100_670_690um_zernike60_00001.tif</t>
-  </si>
-  <si>
     <t>None</t>
   </si>
   <si>
-    <t>Chronic</t>
-  </si>
-  <si>
-    <t>AO-TPLSM</t>
-  </si>
-  <si>
-    <t>Adaptive optic - two photon laser scanning microscope</t>
-  </si>
-  <si>
-    <t>Pantong Industries</t>
-  </si>
-  <si>
-    <t>OpticalChannel2</t>
-  </si>
-  <si>
-    <t>red channel</t>
-  </si>
-  <si>
-    <t>SST+ neuron in layer 5 , 65 focal planes , 100 repeats_for_each_focal plane, system and sample aberration corrected</t>
-  </si>
-  <si>
-    <t>tdTomato</t>
-  </si>
-  <si>
-    <t>barrel cortex</t>
-  </si>
-  <si>
-    <t>(0.1953125, 0.1953125,0.3125)</t>
-  </si>
-  <si>
-    <t>micrometers</t>
-  </si>
-  <si>
     <t>experimenters</t>
   </si>
   <si>
@@ -205,6 +120,114 @@
   </si>
   <si>
     <t>UC San Diego</t>
+  </si>
+  <si>
+    <t>Adaptive optics - two photon laser scanning microscope</t>
+  </si>
+  <si>
+    <t>ROI2_SplC_9x_stk_avg100_670_690um_zernike60_00001</t>
+  </si>
+  <si>
+    <t>age(days)</t>
+  </si>
+  <si>
+    <t>session_start_time(YYYY-MM-DD HH:MM)</t>
+  </si>
+  <si>
+    <t>publication_figures</t>
+  </si>
+  <si>
+    <t>Fig 5, 6</t>
+  </si>
+  <si>
+    <t>description of session</t>
+  </si>
+  <si>
+    <t>AO-TPLSM-7112D</t>
+  </si>
+  <si>
+    <t>Custom</t>
+  </si>
+  <si>
+    <t>acquisition_mode</t>
+  </si>
+  <si>
+    <t>mosaic</t>
+  </si>
+  <si>
+    <t>3d_time_series</t>
+  </si>
+  <si>
+    <t>time_series</t>
+  </si>
+  <si>
+    <t>additional_simultaneous_measurements</t>
+  </si>
+  <si>
+    <t>link_to_additional_measurements</t>
+  </si>
+  <si>
+    <t>z-stack</t>
+  </si>
+  <si>
+    <t>include_nwb</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>surgery_notes</t>
+  </si>
+  <si>
+    <t>chronic</t>
+  </si>
+  <si>
+    <t>pharmacology_notes</t>
+  </si>
+  <si>
+    <t>anesthesize_during_recording</t>
+  </si>
+  <si>
+    <t>optical</t>
+  </si>
+  <si>
+    <t>air-puff</t>
+  </si>
+  <si>
+    <t>mechanical</t>
+  </si>
+  <si>
+    <t>electrical</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>power, mode, wavelength</t>
+  </si>
+  <si>
+    <t>recordings_folder_directory</t>
+  </si>
+  <si>
+    <t>/net/dk-server/pantong/data/Figure 17/ROI2_SplC_9x_stk_avg100_670_690_um_zernike60_00001.xlsx</t>
+  </si>
+  <si>
+    <t>analysis_file</t>
+  </si>
+  <si>
+    <t>notes_file</t>
+  </si>
+  <si>
+    <t>stimulus_notes_file</t>
+  </si>
+  <si>
+    <t>ROI2_SplC_9x_stk_avg100_670_690um_zernike60_00001_D_bBoolsMat.mat</t>
+  </si>
+  <si>
+    <t>ROI2_SplC_9x_stk_avg100_670_690um_zernike60_00001_D_NWBFile_notes.csv</t>
   </si>
 </sst>
 </file>
@@ -249,12 +272,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -342,9 +372,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -382,7 +412,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -488,7 +518,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -630,7 +660,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -638,263 +668,274 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AJ2"/>
+  <dimension ref="A1:AF7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="83.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="4.140625" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" customWidth="1"/>
-    <col min="5" max="5" width="28.140625" customWidth="1"/>
-    <col min="6" max="6" width="5.42578125" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" customWidth="1"/>
-    <col min="10" max="10" width="27" customWidth="1"/>
-    <col min="11" max="11" width="30.85546875" customWidth="1"/>
-    <col min="12" max="12" width="65.140625" customWidth="1"/>
-    <col min="13" max="14" width="20.140625" customWidth="1"/>
-    <col min="15" max="15" width="30.5703125" customWidth="1"/>
-    <col min="16" max="16" width="33.5703125" customWidth="1"/>
-    <col min="17" max="17" width="37.140625" customWidth="1"/>
-    <col min="18" max="18" width="37" customWidth="1"/>
-    <col min="19" max="19" width="16.5703125" customWidth="1"/>
-    <col min="20" max="20" width="18" customWidth="1"/>
-    <col min="21" max="21" width="25.7109375" customWidth="1"/>
-    <col min="22" max="22" width="32.42578125" customWidth="1"/>
-    <col min="23" max="23" width="15.28515625" customWidth="1"/>
-    <col min="26" max="26" width="13.28515625" customWidth="1"/>
-    <col min="27" max="27" width="25.28515625" customWidth="1"/>
-    <col min="28" max="28" width="14" customWidth="1"/>
-    <col min="1024" max="1026" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="59" customWidth="1"/>
+    <col min="2" max="2" width="37.44140625" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1"/>
+    <col min="5" max="5" width="18.5546875" customWidth="1"/>
+    <col min="6" max="6" width="28.109375" customWidth="1"/>
+    <col min="7" max="7" width="5.44140625" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" customWidth="1"/>
+    <col min="10" max="10" width="15.5546875" customWidth="1"/>
+    <col min="11" max="11" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="95.5546875" customWidth="1"/>
+    <col min="14" max="15" width="20.109375" customWidth="1"/>
+    <col min="16" max="16" width="43.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="30.5546875" customWidth="1"/>
+    <col min="18" max="18" width="33.5546875" customWidth="1"/>
+    <col min="19" max="19" width="49.44140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="22.44140625" customWidth="1"/>
+    <col min="21" max="21" width="25.6640625" customWidth="1"/>
+    <col min="22" max="22" width="32.44140625" customWidth="1"/>
+    <col min="23" max="23" width="18.5546875" customWidth="1"/>
+    <col min="24" max="24" width="50.5546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="31" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="52.109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="46" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="39.6640625" style="5" customWidth="1"/>
+    <col min="30" max="30" width="41" style="5" customWidth="1"/>
+    <col min="31" max="31" width="18.6640625" customWidth="1"/>
+    <col min="32" max="32" width="13.44140625" customWidth="1"/>
+    <col min="1016" max="1018" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="S1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="4">
+        <v>45511.583333333336</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2">
         <v>56</v>
       </c>
-      <c r="N1" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="T1" s="1" t="s">
+      <c r="E2" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="F2" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="G2" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="H2" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="I2" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="J2" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="K2" s="2">
+        <v>44783</v>
+      </c>
+      <c r="L2" t="s">
         <v>34</v>
-      </c>
-      <c r="B2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2">
-        <v>56</v>
-      </c>
-      <c r="D2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J2" s="2">
-        <v>44783</v>
-      </c>
-      <c r="K2" t="s">
-        <v>42</v>
-      </c>
-      <c r="L2" t="s">
-        <v>43</v>
       </c>
       <c r="M2" t="s">
         <v>58</v>
       </c>
       <c r="N2" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="O2" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2"/>
+      <c r="Q2" t="s">
+        <v>51</v>
+      </c>
+      <c r="R2" t="s">
+        <v>56</v>
+      </c>
+      <c r="S2" t="s">
+        <v>45</v>
+      </c>
+      <c r="T2" t="s">
+        <v>23</v>
+      </c>
+      <c r="U2" t="s">
+        <v>48</v>
+      </c>
+      <c r="W2" t="s">
+        <v>35</v>
+      </c>
+      <c r="X2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z2" t="s">
         <v>40</v>
       </c>
-      <c r="P2" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>40</v>
-      </c>
-      <c r="R2" t="s">
-        <v>40</v>
-      </c>
-      <c r="S2" t="s">
-        <v>40</v>
-      </c>
-      <c r="T2" t="s">
-        <v>44</v>
-      </c>
-      <c r="U2" t="s">
+      <c r="AC2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF2" t="s">
         <v>45</v>
       </c>
-      <c r="V2">
-        <v>14</v>
-      </c>
-      <c r="W2" t="s">
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="Q3" t="s">
+        <v>54</v>
+      </c>
+      <c r="R3" t="s">
+        <v>55</v>
+      </c>
+      <c r="S3" t="s">
         <v>46</v>
       </c>
-      <c r="X2" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>48</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>50</v>
-      </c>
-      <c r="AB2">
-        <v>593</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>34</v>
-      </c>
-      <c r="AD2">
-        <v>30</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>51</v>
-      </c>
-      <c r="AF2">
-        <v>1030</v>
-      </c>
-      <c r="AG2" t="s">
+      <c r="Z3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="Q4" t="s">
         <v>52</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="Z4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="Q5" t="s">
         <v>53</v>
       </c>
-      <c r="AI2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>55</v>
-      </c>
+      <c r="Z5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="Q7:R7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>